<commit_message>
sắp xếp res theo cột
</commit_message>
<xml_diff>
--- a/danh_sach_san_pham.xlsx
+++ b/danh_sach_san_pham.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\TestSelenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quang/SeleniumMultiCrawler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA7E235-B0D1-44EB-AAB3-FA7099F5CBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20703B33-E43C-3840-A136-D9D9144E3ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5140" yWindow="5460" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sản phẩm" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Barcode</t>
   </si>
@@ -97,34 +97,61 @@
     <t>123456789010</t>
   </si>
   <si>
-    <t>ChocoPIE</t>
-  </si>
-  <si>
-    <t>Danisa</t>
-  </si>
-  <si>
-    <t>Sugus</t>
-  </si>
-  <si>
-    <t>Sweet</t>
-  </si>
-  <si>
-    <t>Milo</t>
-  </si>
-  <si>
-    <t>Ovaltine</t>
-  </si>
-  <si>
-    <t>Dutch Lady</t>
-  </si>
-  <si>
-    <t>Lay's</t>
-  </si>
-  <si>
-    <t>AFC</t>
-  </si>
-  <si>
-    <t>Nabati</t>
+    <t>AMD Ryzen 7 5800X3D</t>
+  </si>
+  <si>
+    <t>GIGABYTE GeForce RTX 4060 Ti EAGLE 8G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corsair Vengeance RS RGB 2x16GB 3600 </t>
+  </si>
+  <si>
+    <t>Asus X570 Rog Crosshair VIII Dark Hero</t>
+  </si>
+  <si>
+    <t>ASUS TUF Gaming 750B - 80 Plus Bronze (750W)</t>
+  </si>
+  <si>
+    <t>SSD WD Black SN850x 1TB M.2 PCIe NVMe Gen 4.0</t>
+  </si>
+  <si>
+    <t>Màn hình cong LG 27GS60QC-B UltraGear 27" 2K 180Hz chuyên game</t>
+  </si>
+  <si>
+    <t>NZXT H5 Flow Black</t>
+  </si>
+  <si>
+    <t>Bộ 3 quạt Corsair RS120 ARGB BLACK (CO-9050181-WW)</t>
+  </si>
+  <si>
+    <t>Cooler Master HYPER 620S</t>
+  </si>
+  <si>
+    <t>Processor</t>
+  </si>
+  <si>
+    <t>Graphics Card</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>Motherboard</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Cooling</t>
   </si>
 </sst>
 </file>
@@ -744,8 +771,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2202F75-B0E6-450E-8583-9F525098E68B}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:F10" xr:uid="{D2202F75-B0E6-450E-8583-9F525098E68B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D2202F75-B0E6-450E-8583-9F525098E68B}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:F11" xr:uid="{D2202F75-B0E6-450E-8583-9F525098E68B}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DF3069DE-9E29-4789-8AFB-5E0A16D20778}" name="Barcode"/>
     <tableColumn id="2" xr3:uid="{8889CAC7-564B-4E60-BF4F-E047095D88AD}" name="Tên MH"/>
@@ -1070,23 +1097,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1106,11 +1133,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="2"/>
@@ -1118,17 +1145,17 @@
         <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="2"/>
@@ -1136,17 +1163,17 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="2"/>
@@ -1154,118 +1181,135 @@
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
+      <c r="B6" t="s">
+        <v>28</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
+      <c r="B7" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F8" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
+      <c r="B9" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
+      <c r="B10" t="s">
+        <v>32</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F10" s="2">
-        <v>6</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1285,14 +1329,14 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1324,14 +1368,14 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1359,7 +1403,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>